<commit_message>
Se realizan mejoras para la version 1
</commit_message>
<xml_diff>
--- a/assets/excelTemplates/PlantillaAppsheetWoocommerce.xlsx
+++ b/assets/excelTemplates/PlantillaAppsheetWoocommerce.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\wordpress-pruebas\wp-content\plugins\wc-appsheet-sync\assets\excelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03FEFB1A-F1F1-48C6-91ED-B03FF948B8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7801E491-259E-4563-9C2E-FD0F7BC684CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="825" windowWidth="22485" windowHeight="14775" xr2:uid="{92E22AB4-F312-4AB2-955A-68FE151DA835}"/>
+    <workbookView xWindow="3525" yWindow="825" windowWidth="22485" windowHeight="14775" activeTab="2" xr2:uid="{92E22AB4-F312-4AB2-955A-68FE151DA835}"/>
   </bookViews>
   <sheets>
     <sheet name="orders" sheetId="1" r:id="rId1"/>
     <sheet name="order_details" sheetId="2" r:id="rId2"/>
+    <sheet name="order_refunds" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -64,6 +65,60 @@
   </si>
   <si>
     <t>quantity</t>
+  </si>
+  <si>
+    <t>address_1</t>
+  </si>
+  <si>
+    <t>address_2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>payment_method</t>
+  </si>
+  <si>
+    <t>payment_method_title</t>
+  </si>
+  <si>
+    <t>discount_total</t>
+  </si>
+  <si>
+    <t>discount_tax</t>
+  </si>
+  <si>
+    <t>shipping_total</t>
+  </si>
+  <si>
+    <t>shipping_tax</t>
+  </si>
+  <si>
+    <t>cart_tax</t>
+  </si>
+  <si>
+    <t>total_tax</t>
+  </si>
+  <si>
+    <t>date_modified</t>
+  </si>
+  <si>
+    <t>reason</t>
   </si>
 </sst>
 </file>
@@ -435,13 +490,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9CAC5E8-02FA-46F3-96CD-599F848B139D}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,13 +506,64 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="U1" t="s">
         <v>4</v>
+      </c>
+      <c r="V1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -496,4 +604,31 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF8D5B41-2AC7-40E8-A8E5-2B4553B0A9F5}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se realizan mejoras para la version pro
</commit_message>
<xml_diff>
--- a/assets/excelTemplates/PlantillaAppsheetWoocommerce.xlsx
+++ b/assets/excelTemplates/PlantillaAppsheetWoocommerce.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\wordpress-pruebas\wp-content\plugins\wc-appsheet-sync\assets\excelTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\wordpress-pruebas\wp-content\plugins\wc_appsheet_sync\assets\excelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7801E491-259E-4563-9C2E-FD0F7BC684CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26B1D12-6669-4B48-AA67-6232144ED232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="825" windowWidth="22485" windowHeight="14775" activeTab="2" xr2:uid="{92E22AB4-F312-4AB2-955A-68FE151DA835}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" activeTab="2" xr2:uid="{92E22AB4-F312-4AB2-955A-68FE151DA835}"/>
   </bookViews>
   <sheets>
     <sheet name="orders" sheetId="1" r:id="rId1"/>
     <sheet name="order_details" sheetId="2" r:id="rId2"/>
     <sheet name="order_refunds" sheetId="3" r:id="rId3"/>
+    <sheet name="products" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>id</t>
   </si>
@@ -119,6 +120,30 @@
   </si>
   <si>
     <t>reason</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>sku</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>regular_price</t>
+  </si>
+  <si>
+    <t>sale_price</t>
+  </si>
+  <si>
+    <t>stock_quantity</t>
+  </si>
+  <si>
+    <t>observaciones</t>
   </si>
 </sst>
 </file>
@@ -492,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9CAC5E8-02FA-46F3-96CD-599F848B139D}">
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +635,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF8D5B41-2AC7-40E8-A8E5-2B4553B0A9F5}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E33:E34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -631,4 +658,57 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B4ECAF4-6E98-4A34-8578-9E70B5662CEF}">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>